<commit_message>
add import file & export file
</commit_message>
<xml_diff>
--- a/InitialFile.xlsx
+++ b/InitialFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jackson\projects\RT7216Q temperature compensation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5C25F3-6D31-440C-95DF-AA25BC2CA105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8A5221-CE53-403B-83E6-8E73C3236B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="36">
   <si>
     <t>max_PWM_chip</t>
   </si>
@@ -141,6 +141,10 @@
   </si>
   <si>
     <t>otp_program_lock</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_PWM_chip</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -472,13 +476,13 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.75" customWidth="1"/>
-    <col min="2" max="2" width="12.625" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,7 +490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -494,7 +498,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -502,7 +506,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -510,7 +514,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -518,7 +522,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -526,7 +530,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -534,7 +538,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -542,7 +546,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -550,7 +554,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -558,7 +562,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -566,7 +570,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -574,7 +578,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -582,7 +586,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -590,7 +594,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -598,7 +602,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -606,7 +610,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -614,7 +618,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -622,7 +626,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -630,7 +634,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -638,7 +642,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -646,7 +650,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -654,7 +658,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -662,7 +666,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -670,7 +674,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -678,7 +682,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -686,7 +690,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -694,7 +698,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -702,7 +706,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -710,7 +714,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -718,7 +722,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>23</v>
       </c>
@@ -726,7 +730,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -734,7 +738,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -742,7 +746,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -750,7 +754,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -769,25 +773,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B7BBFC-8B64-4745-9F13-2A60B4768F2F}">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.75" customWidth="1"/>
-    <col min="2" max="2" width="16.25" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B1">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -795,7 +799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -803,7 +807,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -811,7 +815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -819,7 +823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -827,7 +831,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -835,7 +839,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -843,7 +847,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -851,7 +855,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -859,7 +863,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -867,7 +871,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -875,7 +879,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -883,7 +887,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -891,7 +895,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -899,7 +903,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -907,7 +911,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -915,7 +919,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -923,7 +927,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -931,7 +935,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -939,7 +943,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -947,7 +951,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -955,7 +959,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -963,7 +967,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -971,7 +975,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -979,7 +983,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -987,7 +991,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -995,7 +999,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -1003,7 +1007,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -1011,7 +1015,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -1019,7 +1023,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>23</v>
       </c>
@@ -1027,7 +1031,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -1035,7 +1039,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -1043,7 +1047,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1051,7 +1055,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
revise import non-int value causes crash problem
</commit_message>
<xml_diff>
--- a/InitialFile.xlsx
+++ b/InitialFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jackson\projects\RT7216Q temperature compensation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8A5221-CE53-403B-83E6-8E73C3236B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CD5488-4DB0-4155-A102-C20C1918760D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -773,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B7BBFC-8B64-4745-9F13-2A60B4768F2F}">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -788,7 +788,7 @@
         <v>35</v>
       </c>
       <c r="B1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>